<commit_message>
adding updated classifier scheme
</commit_message>
<xml_diff>
--- a/cms_system_60.xlsx
+++ b/cms_system_60.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A29594C-DBDB-9A4E-B223-935774E11709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535E925A-A9C1-5C45-A0D0-159BBB6D0FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="3580" windowWidth="19320" windowHeight="22340" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26860" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
     <sheet name="Triggers" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Category</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Detector</t>
   </si>
   <si>
-    <t>PU 140</t>
-  </si>
-  <si>
-    <t>PU 200</t>
-  </si>
-  <si>
     <t>Tracking</t>
   </si>
   <si>
@@ -114,18 +108,6 @@
     <t>Data (bytes)</t>
   </si>
   <si>
-    <t>True Pass</t>
-  </si>
-  <si>
-    <t>True Discard</t>
-  </si>
-  <si>
-    <t>False Pass (alpha)</t>
-  </si>
-  <si>
-    <t>False Discard (beta)</t>
-  </si>
-  <si>
     <t>Compression</t>
   </si>
   <si>
@@ -148,6 +130,15 @@
   </si>
   <si>
     <t>Sample Rate</t>
+  </si>
+  <si>
+    <t>Reduction</t>
+  </si>
+  <si>
+    <t>Skill mean</t>
+  </si>
+  <si>
+    <t>Skill variance</t>
   </si>
 </sst>
 </file>
@@ -500,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,7 +503,7 @@
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,33 +511,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>436666.66666666663</v>
@@ -554,28 +530,13 @@
       <c r="D2" s="1">
         <v>40000000</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>206666.66666666669</v>
@@ -583,28 +544,13 @@
       <c r="D3" s="1">
         <v>40000000</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
       <c r="C4">
         <v>126666.66666666669</v>
@@ -612,28 +558,13 @@
       <c r="D4" s="1">
         <v>40000000</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>10000</v>
@@ -641,28 +572,13 @@
       <c r="D5" s="1">
         <v>40000000</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>76666.666666666657</v>
@@ -670,28 +586,13 @@
       <c r="D6" s="1">
         <v>40000000</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
       </c>
       <c r="C7">
         <v>136666.66666666669</v>
@@ -699,28 +600,13 @@
       <c r="D7" s="1">
         <v>40000000</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>180000</v>
@@ -728,28 +614,13 @@
       <c r="D8" s="1">
         <v>40000000</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
       </c>
       <c r="C9">
         <v>240000</v>
@@ -757,28 +628,13 @@
       <c r="D9" s="1">
         <v>40000000</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>30000</v>
@@ -786,28 +642,13 @@
       <c r="D10" s="1">
         <v>40000000</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>60000</v>
@@ -815,28 +656,13 @@
       <c r="D11" s="1">
         <v>40000000</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>56666.666666666672</v>
@@ -844,28 +670,13 @@
       <c r="D12" s="1">
         <v>40000000</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
       </c>
       <c r="C13">
         <v>143333.33333333331</v>
@@ -873,28 +684,13 @@
       <c r="D13" s="1">
         <v>40000000</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>666.66666666666652</v>
@@ -902,28 +698,13 @@
       <c r="D14" s="1">
         <v>40000000</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -931,28 +712,13 @@
       <c r="D15" s="1">
         <v>40000000</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>26666.666666666672</v>
@@ -960,49 +726,19 @@
       <c r="D16" s="1">
         <v>40000000</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>10000</v>
       </c>
       <c r="D17" s="1">
         <v>40000000</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1012,52 +748,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF50D47B-EF5E-D84A-888D-0FD7C5F25128}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1074,16 +801,13 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1100,16 +824,13 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1126,16 +847,13 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1152,75 +870,60 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6">
-        <f>INT(1000000*J6)</f>
-        <v>260000</v>
+        <f>INT(1000000*I6)</f>
+        <v>0</v>
       </c>
       <c r="D6">
+        <v>400</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>399</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0.26</v>
-      </c>
-      <c r="J6">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>99</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1235,9 +938,6 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding gradient results  and environment
</commit_message>
<xml_diff>
--- a/cms_system_60.xlsx
+++ b/cms_system_60.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D763283-4D38-FA4E-A51B-2244C9D33312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA45675-DABE-C643-A95A-6819E3F60711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19640" yWindow="29560" windowWidth="22460" windowHeight="17380" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26800" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>Dummy</t>
   </si>
   <si>
-    <t>Gaussian</t>
-  </si>
-  <si>
     <t>L1T</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>HGCAL TPG Stage2</t>
+  </si>
+  <si>
+    <t>HLT</t>
   </si>
 </sst>
 </file>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,7 +799,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -845,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF50D47B-EF5E-D84A-888D-0FD7C5F25128}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>400</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>

</xml_diff>